<commit_message>
feat: add new information for billing
</commit_message>
<xml_diff>
--- a/public/inscripcion-aguidom.xlsx
+++ b/public/inscripcion-aguidom.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Equipo:</t>
   </si>
@@ -71,6 +71,27 @@
   <si>
     <t>5: (m) 15/16 años: 100</t>
   </si>
+  <si>
+    <t>Pago movil</t>
+  </si>
+  <si>
+    <t>Efectivo</t>
+  </si>
+  <si>
+    <t>Nota: si va a pagar en efectivo coloque el monto total</t>
+  </si>
+  <si>
+    <t>"0191"</t>
+  </si>
+  <si>
+    <t>0426-9599-721</t>
+  </si>
+  <si>
+    <t>30.054.068</t>
+  </si>
+  <si>
+    <t>Nro. De referencia del pago</t>
+  </si>
 </sst>
 </file>
 
@@ -79,11 +100,18 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -106,11 +134,6 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Comic Sans MS"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
       <name val="Comic Sans MS"/>
     </font>
     <font>
@@ -151,6 +174,26 @@
       <name val="Arial Black"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Comic Sans MS"/>
+      <family val="4"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -172,7 +215,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -273,120 +316,190 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -396,10 +509,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -414,6 +527,66 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -707,15 +880,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21.28515625" customWidth="1"/>
     <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" customWidth="1"/>
@@ -727,504 +900,504 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
-      <c r="A1" s="30"/>
-      <c r="B1" s="30"/>
-      <c r="C1" s="31" t="s">
+      <c r="A1" s="26"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="27"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="46"/>
       <c r="J1" s="2"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="15.75">
-      <c r="A2" s="30"/>
-      <c r="B2" s="30"/>
-      <c r="C2" s="31" t="s">
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="46"/>
       <c r="J2" s="2"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="15.75">
-      <c r="A3" s="30"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="31" t="s">
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="27"/>
+      <c r="D3" s="47"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="46"/>
       <c r="J3" s="2"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="15.75">
-      <c r="A4" s="30"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
+      <c r="A4" s="26"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
       <c r="J4" s="2"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="18.75">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="33" t="s">
+      <c r="C5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="33" t="s">
+      <c r="F5" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="33" t="s">
+      <c r="G5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="33" t="s">
+      <c r="H5" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="33" t="s">
+      <c r="I5" s="28" t="s">
         <v>6</v>
       </c>
       <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="33">
+      <c r="A6" s="28">
         <v>1</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="34"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="33">
+      <c r="A7" s="28">
         <v>2</v>
       </c>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="33"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="33">
+      <c r="A8" s="28">
         <v>3</v>
       </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="33">
+      <c r="A9" s="28">
         <v>4</v>
       </c>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="37"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="32"/>
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="33">
+      <c r="A10" s="28">
         <v>5</v>
       </c>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="39"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="34"/>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" s="33">
+      <c r="A11" s="28">
         <v>6</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="36"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="39"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="34"/>
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A12" s="33">
+      <c r="A12" s="28">
         <v>7</v>
       </c>
-      <c r="B12" s="33"/>
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="33"/>
-      <c r="I12" s="41"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="36"/>
       <c r="J12" s="1"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A13" s="33">
+      <c r="A13" s="28">
         <v>8</v>
       </c>
-      <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="33"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="28"/>
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A14" s="33">
+      <c r="A14" s="28">
         <v>9</v>
       </c>
-      <c r="B14" s="33"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="35"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="33"/>
-      <c r="I14" s="33"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
       <c r="J14" s="1"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A15" s="33">
+      <c r="A15" s="28">
         <v>10</v>
       </c>
-      <c r="B15" s="42"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="33"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="28"/>
       <c r="J15" s="1"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A16" s="33">
+      <c r="A16" s="28">
         <v>11</v>
       </c>
-      <c r="B16" s="42"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
       <c r="J16" s="1"/>
     </row>
     <row r="17" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A17" s="33">
+      <c r="A17" s="28">
         <v>12</v>
       </c>
-      <c r="B17" s="33"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="43"/>
-      <c r="F17" s="36"/>
-      <c r="G17" s="36"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
       <c r="J17" s="1"/>
     </row>
     <row r="18" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A18" s="33">
+      <c r="A18" s="28">
         <v>13</v>
       </c>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="33"/>
-      <c r="I18" s="33"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
       <c r="J18" s="1"/>
     </row>
     <row r="19" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A19" s="33">
+      <c r="A19" s="28">
         <v>14</v>
       </c>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="33"/>
-      <c r="I19" s="33"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
       <c r="J19" s="1"/>
     </row>
     <row r="20" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A20" s="33">
+      <c r="A20" s="28">
         <v>15</v>
       </c>
-      <c r="B20" s="33"/>
-      <c r="C20" s="44"/>
-      <c r="D20" s="44"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="44"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="44"/>
-      <c r="I20" s="44"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="39"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="39"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="39"/>
       <c r="J20" s="1"/>
     </row>
     <row r="21" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A21" s="33">
+      <c r="A21" s="28">
         <v>16</v>
       </c>
-      <c r="B21" s="44"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="45"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="44"/>
-      <c r="I21" s="44"/>
+      <c r="B21" s="39"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="39"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39"/>
       <c r="J21" s="1"/>
     </row>
     <row r="22" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A22" s="33">
+      <c r="A22" s="28">
         <v>17</v>
       </c>
-      <c r="B22" s="33"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
       <c r="J22" s="1"/>
     </row>
     <row r="23" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A23" s="33">
+      <c r="A23" s="28">
         <v>18</v>
       </c>
-      <c r="B23" s="42"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="43"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
       <c r="J23" s="1"/>
     </row>
     <row r="24" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A24" s="33">
+      <c r="A24" s="28">
         <v>19</v>
       </c>
-      <c r="B24" s="33"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="33"/>
-      <c r="I24" s="33"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
       <c r="J24" s="1"/>
     </row>
     <row r="25" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A25" s="33">
+      <c r="A25" s="28">
         <v>20</v>
       </c>
-      <c r="B25" s="33"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="36"/>
-      <c r="G25" s="36"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="33"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="28"/>
       <c r="J25" s="1"/>
     </row>
     <row r="26" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A26" s="33">
+      <c r="A26" s="28">
         <v>21</v>
       </c>
-      <c r="B26" s="33"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="33"/>
+      <c r="B26" s="28"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
       <c r="J26" s="1"/>
     </row>
     <row r="27" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A27" s="33">
+      <c r="A27" s="28">
         <v>22</v>
       </c>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
+      <c r="B27" s="39"/>
+      <c r="C27" s="39"/>
+      <c r="D27" s="39"/>
+      <c r="E27" s="40"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="39"/>
+      <c r="I27" s="39"/>
       <c r="J27" s="1"/>
       <c r="L27" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A28" s="33">
+      <c r="A28" s="28">
         <v>23</v>
       </c>
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="35"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="30"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="28"/>
+      <c r="I28" s="28"/>
       <c r="J28" s="1"/>
       <c r="L28" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A29" s="33">
+      <c r="A29" s="28">
         <v>24</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="36"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
+      <c r="B29" s="39"/>
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="41"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="39"/>
+      <c r="I29" s="39"/>
       <c r="J29" s="1"/>
       <c r="L29" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A30" s="33">
+      <c r="A30" s="28">
         <v>25</v>
       </c>
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="43"/>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36"/>
-      <c r="H30" s="42"/>
-      <c r="I30" s="33"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="28"/>
       <c r="J30" s="1"/>
       <c r="L30" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A31" s="33">
+      <c r="A31" s="28">
         <v>26</v>
       </c>
-      <c r="B31" s="42"/>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="36"/>
-      <c r="H31" s="42"/>
-      <c r="I31" s="42"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
       <c r="J31" s="1"/>
       <c r="L31" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="32" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A32" s="33">
+      <c r="A32" s="28">
         <v>27</v>
       </c>
-      <c r="B32" s="42"/>
-      <c r="C32" s="33"/>
-      <c r="D32" s="33"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="36"/>
-      <c r="G32" s="36"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="33"/>
+      <c r="B32" s="37"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="28"/>
+      <c r="I32" s="28"/>
       <c r="J32" s="1"/>
       <c r="L32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15.75" customHeight="1">
-      <c r="A33" s="33">
+      <c r="A33" s="28">
         <v>28</v>
       </c>
-      <c r="B33" s="33"/>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="35"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="33"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="28"/>
+      <c r="I33" s="28"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="1:10" ht="15.75" customHeight="1">
+    <row r="34" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1236,23 +1409,33 @@
       <c r="I34" s="2"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="1:10" ht="15.75" customHeight="1">
+    <row r="35" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
       <c r="A35" s="2"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
+      <c r="B35" s="49" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="D35" s="53" t="s">
+        <v>19</v>
+      </c>
       <c r="E35" s="7"/>
-      <c r="F35" s="8"/>
+      <c r="F35" s="48"/>
       <c r="G35" s="5"/>
-      <c r="H35" s="6"/>
+      <c r="H35" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="I35" s="2"/>
       <c r="J35" s="1"/>
     </row>
     <row r="36" spans="1:10" ht="15.75" customHeight="1">
       <c r="A36" s="2"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
+      <c r="B36" s="63" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="50"/>
+      <c r="D36" s="50"/>
       <c r="E36" s="7"/>
       <c r="F36" s="8"/>
       <c r="G36" s="5"/>
@@ -1262,9 +1445,11 @@
     </row>
     <row r="37" spans="1:10" ht="15.75" customHeight="1">
       <c r="A37" s="2"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
+      <c r="B37" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" s="58"/>
+      <c r="D37" s="58"/>
       <c r="E37" s="7"/>
       <c r="F37" s="8"/>
       <c r="G37" s="5"/>
@@ -1274,10 +1459,12 @@
     </row>
     <row r="38" spans="1:10" ht="15.75" customHeight="1">
       <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="7"/>
+      <c r="B38" s="59" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" s="54"/>
+      <c r="D38" s="54"/>
+      <c r="E38" s="55"/>
       <c r="F38" s="8"/>
       <c r="G38" s="5"/>
       <c r="H38" s="6"/>
@@ -1286,10 +1473,10 @@
     </row>
     <row r="39" spans="1:10" ht="15.75" customHeight="1">
       <c r="A39" s="2"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="7"/>
+      <c r="B39" s="60"/>
+      <c r="C39" s="54"/>
+      <c r="D39" s="54"/>
+      <c r="E39" s="55"/>
       <c r="F39" s="8"/>
       <c r="G39" s="5"/>
       <c r="H39" s="6"/>
@@ -1298,22 +1485,22 @@
     </row>
     <row r="40" spans="1:10" ht="15.75" customHeight="1">
       <c r="A40" s="2"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="11"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="10"/>
-      <c r="I40" s="14"/>
+      <c r="B40" s="61"/>
+      <c r="C40" s="56"/>
+      <c r="D40" s="56"/>
+      <c r="E40" s="57"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="13"/>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="1:10" ht="15.75" customHeight="1">
+    <row r="41" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
       <c r="A41" s="2"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="7"/>
+      <c r="B41" s="62"/>
+      <c r="C41" s="54"/>
+      <c r="D41" s="54"/>
+      <c r="E41" s="55"/>
       <c r="F41" s="8"/>
       <c r="G41" s="5"/>
       <c r="H41" s="6"/>
@@ -1323,9 +1510,9 @@
     <row r="42" spans="1:10" ht="15.75" customHeight="1">
       <c r="A42" s="2"/>
       <c r="B42" s="6"/>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="16"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="15"/>
       <c r="F42" s="8"/>
       <c r="G42" s="5"/>
       <c r="H42" s="2"/>
@@ -1347,30 +1534,30 @@
     <row r="44" spans="1:10" ht="15.75" customHeight="1">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="18"/>
-      <c r="F44" s="17"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="16"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="16"/>
       <c r="G44" s="5"/>
-      <c r="H44" s="17"/>
-      <c r="I44" s="17"/>
+      <c r="H44" s="16"/>
+      <c r="I44" s="16"/>
       <c r="J44" s="1"/>
     </row>
     <row r="45" spans="1:10" ht="15.75" customHeight="1">
       <c r="A45" s="2"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="19"/>
+      <c r="B45" s="16"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="16"/>
+      <c r="E45" s="17"/>
+      <c r="F45" s="18"/>
       <c r="G45" s="5"/>
-      <c r="H45" s="17"/>
-      <c r="I45" s="17"/>
+      <c r="H45" s="16"/>
+      <c r="I45" s="16"/>
       <c r="J45" s="1"/>
     </row>
     <row r="46" spans="1:10" ht="15.75" customHeight="1">
       <c r="A46" s="2"/>
-      <c r="B46" s="20"/>
+      <c r="B46" s="19"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="3"/>
@@ -1382,7 +1569,7 @@
     </row>
     <row r="47" spans="1:10" ht="15.75" customHeight="1">
       <c r="A47" s="2"/>
-      <c r="B47" s="21"/>
+      <c r="B47" s="20"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="3"/>
@@ -1394,14 +1581,14 @@
     </row>
     <row r="48" spans="1:10" ht="15.75" customHeight="1">
       <c r="A48" s="2"/>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="13"/>
-      <c r="H48" s="10"/>
-      <c r="I48" s="14"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="12"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="13"/>
       <c r="J48" s="1"/>
     </row>
     <row r="49" spans="1:11" ht="15.75" customHeight="1">
@@ -1457,7 +1644,7 @@
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
-      <c r="E53" s="22"/>
+      <c r="E53" s="21"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
@@ -1470,7 +1657,7 @@
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
-      <c r="E54" s="22"/>
+      <c r="E54" s="21"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
@@ -1483,7 +1670,7 @@
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
-      <c r="E55" s="22"/>
+      <c r="E55" s="21"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
@@ -1496,7 +1683,7 @@
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
-      <c r="E56" s="22"/>
+      <c r="E56" s="21"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
@@ -1969,7 +2156,7 @@
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
       <c r="I92" s="1"/>
-      <c r="J92" s="23"/>
+      <c r="J92" s="22"/>
     </row>
     <row r="93" spans="1:11" ht="15" customHeight="1">
       <c r="A93" s="1"/>
@@ -1981,7 +2168,7 @@
       <c r="G93" s="1"/>
       <c r="H93" s="1"/>
       <c r="I93" s="1"/>
-      <c r="J93" s="23"/>
+      <c r="J93" s="22"/>
     </row>
     <row r="94" spans="1:11" ht="15" customHeight="1">
       <c r="A94" s="1"/>
@@ -1993,7 +2180,7 @@
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
       <c r="I94" s="1"/>
-      <c r="J94" s="23"/>
+      <c r="J94" s="22"/>
     </row>
     <row r="95" spans="1:11" ht="15" customHeight="1">
       <c r="A95" s="1"/>
@@ -2005,7 +2192,7 @@
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
       <c r="I95" s="1"/>
-      <c r="J95" s="23"/>
+      <c r="J95" s="22"/>
     </row>
     <row r="96" spans="1:11" ht="15.75" customHeight="1"/>
     <row r="97" ht="15.75" customHeight="1"/>

</xml_diff>